<commit_message>
fixed ITS2 output and statistics
</commit_message>
<xml_diff>
--- a/Dec-July-2019-analysis/NCBI_upload/WGBS/WGBS_KBay_SRA_metadata_acc.xlsx
+++ b/Dec-July-2019-analysis/NCBI_upload/WGBS/WGBS_KBay_SRA_metadata_acc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/HI_Bleaching_Timeseries/Dec-July-2019-analysis/NCBI_upload/WGBS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF473EFF-B8C0-E24C-976A-F5B6AA25D102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5406460-9E99-C04B-9D7C-2058910CA95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5600" yWindow="460" windowWidth="28000" windowHeight="19700" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -278,7 +278,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="425">
   <si>
     <t>filename</t>
   </si>
@@ -1338,123 +1338,6 @@
   </si>
   <si>
     <t>DNA methylome from Montipora capitata holobiont (WGBS)</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6001</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6002</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6003</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6004</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6005</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6006</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6007</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6008</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6009</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6010</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6011</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6012</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6013</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6014</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6015</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6016</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6017</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6018</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6019</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6020</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6021</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6022</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6023</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6024</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6025</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6026</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6027</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6028</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6029</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6030</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6031</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6032</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6033</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6034</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6035</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6036</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6037</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6038</t>
-  </si>
-  <si>
-    <t>Illumina NovaSeq 6039</t>
   </si>
   <si>
     <t>WGBS libraries prepared by the Putnam Lab using the Zymo Pico Methyl Seq Library Prep protocol</t>
@@ -2301,6 +2184,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="62"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="62" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2313,16 +2197,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="79">
     <cellStyle name="40% - Accent1" xfId="3" builtinId="31"/>
@@ -2857,52 +2740,52 @@
       </c>
     </row>
     <row r="3" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="40" t="s">
         <v>197</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
     </row>
     <row r="4" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="40" t="s">
         <v>198</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="41" t="s">
         <v>199</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
     </row>
     <row r="6" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
     </row>
     <row r="7" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="22" t="s">
@@ -2962,15 +2845,15 @@
       </c>
     </row>
     <row r="17" spans="2:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
     </row>
     <row r="18" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="19" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3002,27 +2885,27 @@
       <c r="B37" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="C37" s="37" t="s">
+      <c r="C37" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="38"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="C38" s="37" t="s">
+      <c r="C38" s="38" t="s">
         <v>203</v>
       </c>
-      <c r="D38" s="38"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="38"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
     </row>
     <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" s="22" t="s">
@@ -3094,8 +2977,8 @@
   <dimension ref="A1:Q286"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C14" sqref="C14"/>
+      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3175,8 +3058,8 @@
       <c r="A2" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="B2" s="46" t="s">
-        <v>344</v>
+      <c r="B2" s="37" t="s">
+        <v>305</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>303</v>
@@ -3200,24 +3083,24 @@
         <v>247</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K2" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L2" s="46" t="s">
-        <v>384</v>
-      </c>
-      <c r="M2" s="46" t="s">
-        <v>385</v>
+      <c r="L2" s="37" t="s">
+        <v>345</v>
+      </c>
+      <c r="M2" s="37" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="B3" s="46" t="s">
-        <v>345</v>
+      <c r="B3" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>303</v>
@@ -3238,27 +3121,27 @@
         <v>6</v>
       </c>
       <c r="I3" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="J3" s="12" t="s">
         <v>304</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>343</v>
       </c>
       <c r="K3" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L3" s="46" t="s">
-        <v>386</v>
-      </c>
-      <c r="M3" s="46" t="s">
-        <v>387</v>
+      <c r="L3" s="37" t="s">
+        <v>347</v>
+      </c>
+      <c r="M3" s="37" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="B4" s="46" t="s">
-        <v>346</v>
+      <c r="B4" s="37" t="s">
+        <v>307</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>303</v>
@@ -3279,27 +3162,27 @@
         <v>6</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>305</v>
+        <v>247</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K4" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L4" s="46" t="s">
-        <v>388</v>
-      </c>
-      <c r="M4" s="46" t="s">
-        <v>389</v>
+      <c r="L4" s="37" t="s">
+        <v>349</v>
+      </c>
+      <c r="M4" s="37" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>264</v>
       </c>
-      <c r="B5" s="46" t="s">
-        <v>347</v>
+      <c r="B5" s="37" t="s">
+        <v>308</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>303</v>
@@ -3320,27 +3203,27 @@
         <v>6</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>306</v>
+        <v>247</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K5" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L5" s="46" t="s">
-        <v>390</v>
-      </c>
-      <c r="M5" s="46" t="s">
-        <v>391</v>
+      <c r="L5" s="37" t="s">
+        <v>351</v>
+      </c>
+      <c r="M5" s="37" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="B6" s="46" t="s">
-        <v>348</v>
+      <c r="B6" s="37" t="s">
+        <v>309</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>303</v>
@@ -3361,27 +3244,27 @@
         <v>6</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>307</v>
+        <v>247</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L6" s="46" t="s">
-        <v>392</v>
-      </c>
-      <c r="M6" s="46" t="s">
-        <v>393</v>
+      <c r="L6" s="37" t="s">
+        <v>353</v>
+      </c>
+      <c r="M6" s="37" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>266</v>
       </c>
-      <c r="B7" s="46" t="s">
-        <v>349</v>
+      <c r="B7" s="37" t="s">
+        <v>310</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>303</v>
@@ -3402,27 +3285,27 @@
         <v>6</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>308</v>
+        <v>247</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K7" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L7" s="46" t="s">
-        <v>394</v>
-      </c>
-      <c r="M7" s="46" t="s">
-        <v>395</v>
+      <c r="L7" s="37" t="s">
+        <v>355</v>
+      </c>
+      <c r="M7" s="37" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="B8" s="46" t="s">
-        <v>350</v>
+      <c r="B8" s="37" t="s">
+        <v>311</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>303</v>
@@ -3443,27 +3326,27 @@
         <v>6</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>309</v>
+        <v>247</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K8" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L8" s="46" t="s">
-        <v>396</v>
-      </c>
-      <c r="M8" s="46" t="s">
-        <v>397</v>
+      <c r="L8" s="37" t="s">
+        <v>357</v>
+      </c>
+      <c r="M8" s="37" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="B9" s="46" t="s">
-        <v>351</v>
+      <c r="B9" s="37" t="s">
+        <v>312</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>303</v>
@@ -3484,27 +3367,27 @@
         <v>6</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>310</v>
+        <v>247</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K9" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L9" s="46" t="s">
-        <v>398</v>
-      </c>
-      <c r="M9" s="46" t="s">
-        <v>399</v>
+      <c r="L9" s="37" t="s">
+        <v>359</v>
+      </c>
+      <c r="M9" s="37" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>269</v>
       </c>
-      <c r="B10" s="46" t="s">
-        <v>352</v>
+      <c r="B10" s="37" t="s">
+        <v>313</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>303</v>
@@ -3525,27 +3408,27 @@
         <v>6</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>311</v>
+        <v>247</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K10" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L10" s="46" t="s">
-        <v>400</v>
-      </c>
-      <c r="M10" s="46" t="s">
-        <v>401</v>
+      <c r="L10" s="37" t="s">
+        <v>361</v>
+      </c>
+      <c r="M10" s="37" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="B11" s="46" t="s">
-        <v>353</v>
+      <c r="B11" s="37" t="s">
+        <v>314</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>303</v>
@@ -3566,27 +3449,27 @@
         <v>6</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>312</v>
+        <v>247</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K11" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L11" s="46" t="s">
-        <v>402</v>
-      </c>
-      <c r="M11" s="46" t="s">
-        <v>403</v>
+      <c r="L11" s="37" t="s">
+        <v>363</v>
+      </c>
+      <c r="M11" s="37" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>271</v>
       </c>
-      <c r="B12" s="46" t="s">
-        <v>354</v>
+      <c r="B12" s="37" t="s">
+        <v>315</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>303</v>
@@ -3607,27 +3490,27 @@
         <v>6</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>313</v>
+        <v>247</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K12" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L12" s="46" t="s">
-        <v>404</v>
-      </c>
-      <c r="M12" s="46" t="s">
-        <v>405</v>
+      <c r="L12" s="37" t="s">
+        <v>365</v>
+      </c>
+      <c r="M12" s="37" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="B13" s="46" t="s">
-        <v>355</v>
+      <c r="B13" s="37" t="s">
+        <v>316</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>303</v>
@@ -3648,27 +3531,27 @@
         <v>6</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>314</v>
+        <v>247</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K13" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L13" s="46" t="s">
-        <v>406</v>
-      </c>
-      <c r="M13" s="46" t="s">
-        <v>407</v>
+      <c r="L13" s="37" t="s">
+        <v>367</v>
+      </c>
+      <c r="M13" s="37" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="B14" s="46" t="s">
-        <v>356</v>
+      <c r="B14" s="37" t="s">
+        <v>317</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>303</v>
@@ -3689,27 +3572,27 @@
         <v>6</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>315</v>
+        <v>247</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K14" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L14" s="46" t="s">
-        <v>408</v>
-      </c>
-      <c r="M14" s="46" t="s">
-        <v>409</v>
+      <c r="L14" s="37" t="s">
+        <v>369</v>
+      </c>
+      <c r="M14" s="37" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="B15" s="46" t="s">
-        <v>357</v>
+      <c r="B15" s="37" t="s">
+        <v>318</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>303</v>
@@ -3730,27 +3613,27 @@
         <v>6</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>316</v>
+        <v>247</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K15" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L15" s="46" t="s">
-        <v>410</v>
-      </c>
-      <c r="M15" s="46" t="s">
-        <v>411</v>
+      <c r="L15" s="37" t="s">
+        <v>371</v>
+      </c>
+      <c r="M15" s="37" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="B16" s="46" t="s">
-        <v>358</v>
+      <c r="B16" s="37" t="s">
+        <v>319</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>303</v>
@@ -3771,27 +3654,27 @@
         <v>6</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>317</v>
+        <v>247</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K16" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L16" s="46" t="s">
-        <v>412</v>
-      </c>
-      <c r="M16" s="46" t="s">
-        <v>413</v>
+      <c r="L16" s="37" t="s">
+        <v>373</v>
+      </c>
+      <c r="M16" s="37" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>276</v>
       </c>
-      <c r="B17" s="46" t="s">
-        <v>359</v>
+      <c r="B17" s="37" t="s">
+        <v>320</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>303</v>
@@ -3812,27 +3695,27 @@
         <v>6</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>318</v>
+        <v>247</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K17" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L17" s="46" t="s">
-        <v>414</v>
-      </c>
-      <c r="M17" s="46" t="s">
-        <v>415</v>
+      <c r="L17" s="37" t="s">
+        <v>375</v>
+      </c>
+      <c r="M17" s="37" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="B18" s="46" t="s">
-        <v>360</v>
+      <c r="B18" s="37" t="s">
+        <v>321</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>303</v>
@@ -3853,27 +3736,27 @@
         <v>6</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>319</v>
+        <v>247</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K18" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L18" s="46" t="s">
-        <v>416</v>
-      </c>
-      <c r="M18" s="46" t="s">
-        <v>417</v>
+      <c r="L18" s="37" t="s">
+        <v>377</v>
+      </c>
+      <c r="M18" s="37" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="B19" s="46" t="s">
-        <v>361</v>
+      <c r="B19" s="37" t="s">
+        <v>322</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>303</v>
@@ -3894,27 +3777,27 @@
         <v>6</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>320</v>
+        <v>247</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K19" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L19" s="46" t="s">
-        <v>418</v>
-      </c>
-      <c r="M19" s="46" t="s">
-        <v>419</v>
+      <c r="L19" s="37" t="s">
+        <v>379</v>
+      </c>
+      <c r="M19" s="37" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="B20" s="46" t="s">
-        <v>362</v>
+      <c r="B20" s="37" t="s">
+        <v>323</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>303</v>
@@ -3935,27 +3818,27 @@
         <v>6</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>321</v>
+        <v>247</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K20" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L20" s="46" t="s">
-        <v>420</v>
-      </c>
-      <c r="M20" s="46" t="s">
-        <v>421</v>
+      <c r="L20" s="37" t="s">
+        <v>381</v>
+      </c>
+      <c r="M20" s="37" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="B21" s="46" t="s">
-        <v>363</v>
+      <c r="B21" s="37" t="s">
+        <v>324</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>303</v>
@@ -3976,27 +3859,27 @@
         <v>6</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>322</v>
+        <v>247</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K21" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L21" s="46" t="s">
-        <v>422</v>
-      </c>
-      <c r="M21" s="46" t="s">
-        <v>423</v>
+      <c r="L21" s="37" t="s">
+        <v>383</v>
+      </c>
+      <c r="M21" s="37" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="B22" s="46" t="s">
-        <v>364</v>
+      <c r="B22" s="37" t="s">
+        <v>325</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>303</v>
@@ -4017,27 +3900,27 @@
         <v>6</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>323</v>
+        <v>247</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K22" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L22" s="46" t="s">
-        <v>424</v>
-      </c>
-      <c r="M22" s="46" t="s">
-        <v>425</v>
+      <c r="L22" s="37" t="s">
+        <v>385</v>
+      </c>
+      <c r="M22" s="37" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="B23" s="46" t="s">
-        <v>365</v>
+      <c r="B23" s="37" t="s">
+        <v>326</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>303</v>
@@ -4058,27 +3941,27 @@
         <v>6</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>324</v>
+        <v>247</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K23" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L23" s="46" t="s">
-        <v>426</v>
-      </c>
-      <c r="M23" s="46" t="s">
-        <v>427</v>
+      <c r="L23" s="37" t="s">
+        <v>387</v>
+      </c>
+      <c r="M23" s="37" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="B24" s="46" t="s">
-        <v>366</v>
+      <c r="B24" s="37" t="s">
+        <v>327</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>303</v>
@@ -4099,27 +3982,27 @@
         <v>6</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>325</v>
+        <v>247</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K24" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L24" s="46" t="s">
-        <v>428</v>
-      </c>
-      <c r="M24" s="46" t="s">
-        <v>429</v>
+      <c r="L24" s="37" t="s">
+        <v>389</v>
+      </c>
+      <c r="M24" s="37" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
         <v>284</v>
       </c>
-      <c r="B25" s="46" t="s">
-        <v>367</v>
+      <c r="B25" s="37" t="s">
+        <v>328</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>303</v>
@@ -4140,27 +4023,27 @@
         <v>6</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>326</v>
+        <v>247</v>
       </c>
       <c r="J25" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K25" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L25" s="46" t="s">
-        <v>430</v>
-      </c>
-      <c r="M25" s="46" t="s">
-        <v>431</v>
+      <c r="L25" s="37" t="s">
+        <v>391</v>
+      </c>
+      <c r="M25" s="37" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="B26" s="46" t="s">
-        <v>368</v>
+      <c r="B26" s="37" t="s">
+        <v>329</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>303</v>
@@ -4181,27 +4064,27 @@
         <v>6</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>327</v>
+        <v>247</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K26" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L26" s="46" t="s">
-        <v>432</v>
-      </c>
-      <c r="M26" s="46" t="s">
-        <v>433</v>
+      <c r="L26" s="37" t="s">
+        <v>393</v>
+      </c>
+      <c r="M26" s="37" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="B27" s="46" t="s">
-        <v>369</v>
+      <c r="B27" s="37" t="s">
+        <v>330</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>303</v>
@@ -4222,27 +4105,27 @@
         <v>6</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>328</v>
+        <v>247</v>
       </c>
       <c r="J27" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K27" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L27" s="46" t="s">
-        <v>434</v>
-      </c>
-      <c r="M27" s="46" t="s">
-        <v>435</v>
+      <c r="L27" s="37" t="s">
+        <v>395</v>
+      </c>
+      <c r="M27" s="37" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
         <v>287</v>
       </c>
-      <c r="B28" s="46" t="s">
-        <v>370</v>
+      <c r="B28" s="37" t="s">
+        <v>331</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>303</v>
@@ -4263,27 +4146,27 @@
         <v>6</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>329</v>
+        <v>247</v>
       </c>
       <c r="J28" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K28" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L28" s="46" t="s">
-        <v>436</v>
-      </c>
-      <c r="M28" s="46" t="s">
-        <v>437</v>
+      <c r="L28" s="37" t="s">
+        <v>397</v>
+      </c>
+      <c r="M28" s="37" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>288</v>
       </c>
-      <c r="B29" s="46" t="s">
-        <v>371</v>
+      <c r="B29" s="37" t="s">
+        <v>332</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>303</v>
@@ -4304,27 +4187,27 @@
         <v>6</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>330</v>
+        <v>247</v>
       </c>
       <c r="J29" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K29" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L29" s="46" t="s">
-        <v>438</v>
-      </c>
-      <c r="M29" s="46" t="s">
-        <v>439</v>
+      <c r="L29" s="37" t="s">
+        <v>399</v>
+      </c>
+      <c r="M29" s="37" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>289</v>
       </c>
-      <c r="B30" s="46" t="s">
-        <v>372</v>
+      <c r="B30" s="37" t="s">
+        <v>333</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>303</v>
@@ -4345,27 +4228,27 @@
         <v>6</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>331</v>
+        <v>247</v>
       </c>
       <c r="J30" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K30" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L30" s="46" t="s">
-        <v>440</v>
-      </c>
-      <c r="M30" s="46" t="s">
-        <v>441</v>
+      <c r="L30" s="37" t="s">
+        <v>401</v>
+      </c>
+      <c r="M30" s="37" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
         <v>290</v>
       </c>
-      <c r="B31" s="46" t="s">
-        <v>373</v>
+      <c r="B31" s="37" t="s">
+        <v>334</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>303</v>
@@ -4386,27 +4269,27 @@
         <v>6</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>332</v>
+        <v>247</v>
       </c>
       <c r="J31" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K31" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L31" s="46" t="s">
-        <v>442</v>
-      </c>
-      <c r="M31" s="46" t="s">
-        <v>443</v>
+      <c r="L31" s="37" t="s">
+        <v>403</v>
+      </c>
+      <c r="M31" s="37" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
         <v>291</v>
       </c>
-      <c r="B32" s="46" t="s">
-        <v>374</v>
+      <c r="B32" s="37" t="s">
+        <v>335</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>303</v>
@@ -4427,27 +4310,27 @@
         <v>6</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>333</v>
+        <v>247</v>
       </c>
       <c r="J32" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K32" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L32" s="46" t="s">
-        <v>444</v>
-      </c>
-      <c r="M32" s="46" t="s">
-        <v>445</v>
+      <c r="L32" s="37" t="s">
+        <v>405</v>
+      </c>
+      <c r="M32" s="37" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
         <v>292</v>
       </c>
-      <c r="B33" s="46" t="s">
-        <v>375</v>
+      <c r="B33" s="37" t="s">
+        <v>336</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>303</v>
@@ -4468,27 +4351,27 @@
         <v>6</v>
       </c>
       <c r="I33" s="11" t="s">
-        <v>334</v>
+        <v>247</v>
       </c>
       <c r="J33" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K33" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L33" s="46" t="s">
-        <v>446</v>
-      </c>
-      <c r="M33" s="46" t="s">
-        <v>447</v>
+      <c r="L33" s="37" t="s">
+        <v>407</v>
+      </c>
+      <c r="M33" s="37" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
         <v>293</v>
       </c>
-      <c r="B34" s="46" t="s">
-        <v>376</v>
+      <c r="B34" s="37" t="s">
+        <v>337</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>303</v>
@@ -4509,27 +4392,27 @@
         <v>6</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>335</v>
+        <v>247</v>
       </c>
       <c r="J34" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K34" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L34" s="46" t="s">
-        <v>448</v>
-      </c>
-      <c r="M34" s="46" t="s">
-        <v>449</v>
+      <c r="L34" s="37" t="s">
+        <v>409</v>
+      </c>
+      <c r="M34" s="37" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
         <v>294</v>
       </c>
-      <c r="B35" s="46" t="s">
-        <v>377</v>
+      <c r="B35" s="37" t="s">
+        <v>338</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>303</v>
@@ -4550,27 +4433,27 @@
         <v>6</v>
       </c>
       <c r="I35" s="11" t="s">
-        <v>336</v>
+        <v>247</v>
       </c>
       <c r="J35" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K35" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L35" s="46" t="s">
-        <v>450</v>
-      </c>
-      <c r="M35" s="46" t="s">
-        <v>451</v>
+      <c r="L35" s="37" t="s">
+        <v>411</v>
+      </c>
+      <c r="M35" s="37" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
         <v>295</v>
       </c>
-      <c r="B36" s="46" t="s">
-        <v>378</v>
+      <c r="B36" s="37" t="s">
+        <v>339</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>303</v>
@@ -4591,27 +4474,27 @@
         <v>6</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>337</v>
+        <v>247</v>
       </c>
       <c r="J36" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K36" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L36" s="46" t="s">
-        <v>452</v>
-      </c>
-      <c r="M36" s="46" t="s">
-        <v>453</v>
+      <c r="L36" s="37" t="s">
+        <v>413</v>
+      </c>
+      <c r="M36" s="37" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
         <v>296</v>
       </c>
-      <c r="B37" s="46" t="s">
-        <v>379</v>
+      <c r="B37" s="37" t="s">
+        <v>340</v>
       </c>
       <c r="C37" s="13" t="s">
         <v>303</v>
@@ -4632,27 +4515,27 @@
         <v>6</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>338</v>
+        <v>247</v>
       </c>
       <c r="J37" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K37" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L37" s="46" t="s">
-        <v>454</v>
-      </c>
-      <c r="M37" s="46" t="s">
-        <v>455</v>
+      <c r="L37" s="37" t="s">
+        <v>415</v>
+      </c>
+      <c r="M37" s="37" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
         <v>297</v>
       </c>
-      <c r="B38" s="46" t="s">
-        <v>380</v>
+      <c r="B38" s="37" t="s">
+        <v>341</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>303</v>
@@ -4673,27 +4556,27 @@
         <v>6</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>339</v>
+        <v>247</v>
       </c>
       <c r="J38" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K38" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L38" s="46" t="s">
-        <v>456</v>
-      </c>
-      <c r="M38" s="46" t="s">
-        <v>457</v>
+      <c r="L38" s="37" t="s">
+        <v>417</v>
+      </c>
+      <c r="M38" s="37" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
         <v>298</v>
       </c>
-      <c r="B39" s="46" t="s">
-        <v>381</v>
+      <c r="B39" s="37" t="s">
+        <v>342</v>
       </c>
       <c r="C39" s="13" t="s">
         <v>303</v>
@@ -4714,27 +4597,27 @@
         <v>6</v>
       </c>
       <c r="I39" s="11" t="s">
-        <v>340</v>
+        <v>247</v>
       </c>
       <c r="J39" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K39" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L39" s="46" t="s">
-        <v>458</v>
-      </c>
-      <c r="M39" s="46" t="s">
-        <v>459</v>
+      <c r="L39" s="37" t="s">
+        <v>419</v>
+      </c>
+      <c r="M39" s="37" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
         <v>299</v>
       </c>
-      <c r="B40" s="46" t="s">
-        <v>382</v>
+      <c r="B40" s="37" t="s">
+        <v>343</v>
       </c>
       <c r="C40" s="13" t="s">
         <v>303</v>
@@ -4755,27 +4638,27 @@
         <v>6</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>341</v>
+        <v>247</v>
       </c>
       <c r="J40" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K40" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L40" s="46" t="s">
-        <v>460</v>
-      </c>
-      <c r="M40" s="46" t="s">
-        <v>461</v>
+      <c r="L40" s="37" t="s">
+        <v>421</v>
+      </c>
+      <c r="M40" s="37" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
         <v>300</v>
       </c>
-      <c r="B41" s="46" t="s">
-        <v>383</v>
+      <c r="B41" s="37" t="s">
+        <v>344</v>
       </c>
       <c r="C41" s="13" t="s">
         <v>303</v>
@@ -4796,19 +4679,19 @@
         <v>6</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>342</v>
+        <v>247</v>
       </c>
       <c r="J41" s="12" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="K41" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="L41" s="46" t="s">
-        <v>462</v>
-      </c>
-      <c r="M41" s="46" t="s">
-        <v>463</v>
+      <c r="L41" s="37" t="s">
+        <v>423</v>
+      </c>
+      <c r="M41" s="37" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
@@ -7080,15 +6963,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
     </row>
     <row r="2" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="44"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -7100,172 +6983,172 @@
       <c r="A3" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="42"/>
+      <c r="C3" s="43"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="42"/>
+      <c r="C4" s="43"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="42"/>
+      <c r="C5" s="43"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="C6" s="42"/>
+      <c r="C6" s="43"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="42"/>
+      <c r="C7" s="43"/>
     </row>
     <row r="8" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="42"/>
+      <c r="C8" s="43"/>
     </row>
     <row r="9" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="42"/>
+      <c r="C9" s="43"/>
     </row>
     <row r="10" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="C10" s="42"/>
+      <c r="C10" s="43"/>
     </row>
     <row r="11" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="42"/>
+      <c r="C11" s="43"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="C12" s="42"/>
+      <c r="C12" s="43"/>
     </row>
     <row r="13" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="42"/>
+      <c r="C13" s="43"/>
     </row>
     <row r="14" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="42"/>
+      <c r="C14" s="43"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="42"/>
+      <c r="C15" s="43"/>
     </row>
     <row r="16" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="C16" s="42"/>
+      <c r="C16" s="43"/>
     </row>
     <row r="17" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="C17" s="42"/>
+      <c r="C17" s="43"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="C18" s="42"/>
+      <c r="C18" s="43"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="C19" s="42"/>
+      <c r="C19" s="43"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="C20" s="42"/>
+      <c r="C20" s="43"/>
     </row>
     <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A21" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C21" s="42"/>
+      <c r="C21" s="43"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -7277,28 +7160,28 @@
       <c r="A22" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="C22" s="42"/>
+      <c r="C22" s="43"/>
     </row>
     <row r="23" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="C23" s="42"/>
+      <c r="C23" s="43"/>
     </row>
     <row r="24" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="43" t="s">
         <v>131</v>
       </c>
-      <c r="C24" s="42"/>
+      <c r="C24" s="43"/>
     </row>
     <row r="25" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
@@ -7402,75 +7285,75 @@
       <c r="A37" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B37" s="42" t="s">
+      <c r="B37" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="C37" s="42"/>
+      <c r="C37" s="43"/>
     </row>
     <row r="38" spans="1:3" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="42"/>
-      <c r="C38" s="42"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="43"/>
     </row>
     <row r="39" spans="1:3" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A39" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="43"/>
-      <c r="C39" s="44"/>
+      <c r="B39" s="45"/>
+      <c r="C39" s="46"/>
     </row>
     <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="B40" s="42" t="s">
+      <c r="B40" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="C40" s="42"/>
+      <c r="C40" s="43"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="B41" s="42" t="s">
+      <c r="B41" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="C41" s="42"/>
+      <c r="C41" s="43"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="B42" s="42" t="s">
+      <c r="B42" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="C42" s="42"/>
+      <c r="C42" s="43"/>
     </row>
     <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="B43" s="42" t="s">
+      <c r="B43" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="C43" s="42"/>
+      <c r="C43" s="43"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="B44" s="42" t="s">
+      <c r="B44" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="C44" s="42"/>
+      <c r="C44" s="43"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="B45" s="42" t="s">
+      <c r="B45" s="43" t="s">
         <v>138</v>
       </c>
-      <c r="C45" s="42"/>
+      <c r="C45" s="43"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
@@ -7486,264 +7369,264 @@
       <c r="A48" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B48" s="42" t="s">
+      <c r="B48" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="C48" s="42"/>
+      <c r="C48" s="43"/>
     </row>
     <row r="49" spans="1:3" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="42"/>
-      <c r="C49" s="42"/>
+      <c r="B49" s="43"/>
+      <c r="C49" s="43"/>
     </row>
     <row r="50" spans="1:3" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A50" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B50" s="45"/>
-      <c r="C50" s="42"/>
+      <c r="B50" s="44"/>
+      <c r="C50" s="43"/>
     </row>
     <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="B51" s="42" t="s">
+      <c r="B51" s="43" t="s">
         <v>140</v>
       </c>
-      <c r="C51" s="42"/>
+      <c r="C51" s="43"/>
     </row>
     <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="B52" s="42" t="s">
+      <c r="B52" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="C52" s="42"/>
+      <c r="C52" s="43"/>
     </row>
     <row r="53" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="B53" s="42" t="s">
+      <c r="B53" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="C53" s="42"/>
+      <c r="C53" s="43"/>
     </row>
     <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="B54" s="42" t="s">
+      <c r="B54" s="43" t="s">
         <v>143</v>
       </c>
-      <c r="C54" s="42"/>
+      <c r="C54" s="43"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A55" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="B55" s="42" t="s">
+      <c r="B55" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="C55" s="42"/>
+      <c r="C55" s="43"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A56" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="B56" s="42" t="s">
+      <c r="B56" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="C56" s="42"/>
+      <c r="C56" s="43"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A57" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B57" s="42" t="s">
+      <c r="B57" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="C57" s="42"/>
+      <c r="C57" s="43"/>
     </row>
     <row r="58" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="B58" s="42" t="s">
+      <c r="B58" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="C58" s="42"/>
+      <c r="C58" s="43"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A59" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="B59" s="42" t="s">
+      <c r="B59" s="43" t="s">
         <v>148</v>
       </c>
-      <c r="C59" s="42"/>
+      <c r="C59" s="43"/>
     </row>
     <row r="60" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="B60" s="42" t="s">
+      <c r="B60" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="C60" s="42"/>
+      <c r="C60" s="43"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A61" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="B61" s="42" t="s">
+      <c r="B61" s="43" t="s">
         <v>150</v>
       </c>
-      <c r="C61" s="42"/>
+      <c r="C61" s="43"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A62" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="B62" s="42" t="s">
+      <c r="B62" s="43" t="s">
         <v>151</v>
       </c>
-      <c r="C62" s="42"/>
+      <c r="C62" s="43"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A63" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="B63" s="42" t="s">
+      <c r="B63" s="43" t="s">
         <v>152</v>
       </c>
-      <c r="C63" s="42"/>
+      <c r="C63" s="43"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A64" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="B64" s="42" t="s">
+      <c r="B64" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="C64" s="42"/>
+      <c r="C64" s="43"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A65" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="B65" s="42" t="s">
+      <c r="B65" s="43" t="s">
         <v>154</v>
       </c>
-      <c r="C65" s="42"/>
+      <c r="C65" s="43"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A66" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="B66" s="42" t="s">
+      <c r="B66" s="43" t="s">
         <v>155</v>
       </c>
-      <c r="C66" s="42"/>
+      <c r="C66" s="43"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A67" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B67" s="42" t="s">
+      <c r="B67" s="43" t="s">
         <v>156</v>
       </c>
-      <c r="C67" s="42"/>
+      <c r="C67" s="43"/>
     </row>
     <row r="68" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="B68" s="42" t="s">
+      <c r="B68" s="43" t="s">
         <v>157</v>
       </c>
-      <c r="C68" s="42"/>
+      <c r="C68" s="43"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A69" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="B69" s="42" t="s">
+      <c r="B69" s="43" t="s">
         <v>158</v>
       </c>
-      <c r="C69" s="42"/>
+      <c r="C69" s="43"/>
     </row>
     <row r="70" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="B70" s="42" t="s">
+      <c r="B70" s="43" t="s">
         <v>159</v>
       </c>
-      <c r="C70" s="42"/>
+      <c r="C70" s="43"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A71" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="B71" s="42" t="s">
+      <c r="B71" s="43" t="s">
         <v>160</v>
       </c>
-      <c r="C71" s="42"/>
+      <c r="C71" s="43"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A72" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B72" s="42" t="s">
+      <c r="B72" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="C72" s="42"/>
+      <c r="C72" s="43"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A73" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="B73" s="42" t="s">
+      <c r="B73" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="C73" s="42"/>
+      <c r="C73" s="43"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A74" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="B74" s="42" t="s">
+      <c r="B74" s="43" t="s">
         <v>163</v>
       </c>
-      <c r="C74" s="42"/>
+      <c r="C74" s="43"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A75" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="B75" s="42" t="s">
+      <c r="B75" s="43" t="s">
         <v>164</v>
       </c>
-      <c r="C75" s="42"/>
+      <c r="C75" s="43"/>
     </row>
     <row r="76" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="B76" s="42" t="s">
+      <c r="B76" s="43" t="s">
         <v>165</v>
       </c>
-      <c r="C76" s="42"/>
+      <c r="C76" s="43"/>
     </row>
     <row r="77" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B77" s="42" t="s">
+      <c r="B77" s="43" t="s">
         <v>166</v>
       </c>
-      <c r="C77" s="42"/>
+      <c r="C77" s="43"/>
     </row>
     <row r="78" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="2" t="s">
@@ -8096,15 +7979,48 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
     <mergeCell ref="B68:C68"/>
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="B58:C58"/>
@@ -8117,48 +8033,15 @@
     <mergeCell ref="B65:C65"/>
     <mergeCell ref="B66:C66"/>
     <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>